<commit_message>
add 2022 song data
</commit_message>
<xml_diff>
--- a/data/cabin_music_2022.xlsx
+++ b/data/cabin_music_2022.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2814" uniqueCount="963">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3184" uniqueCount="1082">
   <si>
     <t>friend</t>
   </si>
@@ -186,7 +186,7 @@
     <t>Woman</t>
   </si>
   <si>
-    <t>Woflmother</t>
+    <t>Wolfmother</t>
   </si>
   <si>
     <t>JZ</t>
@@ -279,13 +279,13 @@
     <t>Pumped up Kicks (Acoustic)</t>
   </si>
   <si>
-    <t>Tonight (I'm Fuckin' You)</t>
+    <t>Tonight (I'm Lovin' You)</t>
   </si>
   <si>
     <t>Enrique Iglasias ft Ludacris</t>
   </si>
   <si>
-    <t>How do you Sleep?</t>
+    <t>How Do You Sleep?</t>
   </si>
   <si>
     <t>Jesse McCartney ft Ludacris</t>
@@ -327,7 +327,7 @@
     <t>MGMT</t>
   </si>
   <si>
-    <t>Jump (For my Love)</t>
+    <t>Jump (For My Love)</t>
   </si>
   <si>
     <t>The Pointer Sisters</t>
@@ -363,13 +363,13 @@
     <t>Yuck</t>
   </si>
   <si>
-    <t>Where is my Mind?</t>
+    <t>Where is My Mind?</t>
   </si>
   <si>
     <t>Pixies</t>
   </si>
   <si>
-    <t>Objects of my Affection</t>
+    <t>Objects of My Affection</t>
   </si>
   <si>
     <t>I Wanna Know About U</t>
@@ -411,7 +411,7 @@
     <t>Lillian, Egypt</t>
   </si>
   <si>
-    <t>JZ Ritter</t>
+    <t>Josh Ritter</t>
   </si>
   <si>
     <t>Medication</t>
@@ -2229,7 +2229,7 @@
     <t>a-ha</t>
   </si>
   <si>
-    <t>Nick Murphy / Chet Faker</t>
+    <t>Chet Faker</t>
   </si>
   <si>
     <t>Live in the Moment</t>
@@ -2853,9 +2853,6 @@
     <t>Low</t>
   </si>
   <si>
-    <t>Chet Faker</t>
-  </si>
-  <si>
     <t>Karaoke</t>
   </si>
   <si>
@@ -2905,6 +2902,366 @@
   </si>
   <si>
     <t>Dayglow</t>
+  </si>
+  <si>
+    <t>Save Your Tears</t>
+  </si>
+  <si>
+    <t>Merry New Plague (2022)</t>
+  </si>
+  <si>
+    <t>So Hot You're Hurting My Feelings</t>
+  </si>
+  <si>
+    <t>Caroline Polachek</t>
+  </si>
+  <si>
+    <t>Poets</t>
+  </si>
+  <si>
+    <t>The Rock Show</t>
+  </si>
+  <si>
+    <t>Back of the Car</t>
+  </si>
+  <si>
+    <t>Watermelon Sugar</t>
+  </si>
+  <si>
+    <t>Harry Styles</t>
+  </si>
+  <si>
+    <t>Big Energy</t>
+  </si>
+  <si>
+    <t>Latto</t>
+  </si>
+  <si>
+    <t>I AM WOMAN</t>
+  </si>
+  <si>
+    <t>Emmy Meli</t>
+  </si>
+  <si>
+    <t>Cloudy Day</t>
+  </si>
+  <si>
+    <t>Tones And I</t>
+  </si>
+  <si>
+    <t>Let's go to Hell</t>
+  </si>
+  <si>
+    <t>Tai Verdes</t>
+  </si>
+  <si>
+    <t>They Say I'm Different</t>
+  </si>
+  <si>
+    <t>Betty Davis</t>
+  </si>
+  <si>
+    <t>Clint Eastwood</t>
+  </si>
+  <si>
+    <t>Gorillaz</t>
+  </si>
+  <si>
+    <t>I'm A Lady</t>
+  </si>
+  <si>
+    <t>Santigold ft Trouble Andrew</t>
+  </si>
+  <si>
+    <t>Gimme! Gimme! Gimme! (A Man After Midnight)</t>
+  </si>
+  <si>
+    <t>Kick It to Me</t>
+  </si>
+  <si>
+    <t>Sammy Rae &amp; The Friends</t>
+  </si>
+  <si>
+    <t>Black Water</t>
+  </si>
+  <si>
+    <t>The Doobie Brothers</t>
+  </si>
+  <si>
+    <t>Dancing in the Moonlight</t>
+  </si>
+  <si>
+    <t>King Harvest</t>
+  </si>
+  <si>
+    <t>Music For a Sushi Restaurant</t>
+  </si>
+  <si>
+    <t>edamame</t>
+  </si>
+  <si>
+    <t>bbno$ ft Rich Brian</t>
+  </si>
+  <si>
+    <t>If It Makes You Happy</t>
+  </si>
+  <si>
+    <t>Sheryl Crow</t>
+  </si>
+  <si>
+    <t>Hannah Sun</t>
+  </si>
+  <si>
+    <t>Lomelda</t>
+  </si>
+  <si>
+    <t>Smokin Out The Window</t>
+  </si>
+  <si>
+    <t>Bruno Mars ft Anderson .Paak, Silk Sonic</t>
+  </si>
+  <si>
+    <t>Invisible Touch</t>
+  </si>
+  <si>
+    <t>Genesis</t>
+  </si>
+  <si>
+    <t>Working in the Coal Mine</t>
+  </si>
+  <si>
+    <t>DEVO</t>
+  </si>
+  <si>
+    <t>Never Ending Game - Panda Bear Remix</t>
+  </si>
+  <si>
+    <t>Angel Du$t ft Panda Bear</t>
+  </si>
+  <si>
+    <t>For Whom The Bell Tolls</t>
+  </si>
+  <si>
+    <t>Metallica</t>
+  </si>
+  <si>
+    <t>DDAJ</t>
+  </si>
+  <si>
+    <t>Heat Waves</t>
+  </si>
+  <si>
+    <t>Feels Like Summer</t>
+  </si>
+  <si>
+    <t>Chapstick</t>
+  </si>
+  <si>
+    <t>COIN</t>
+  </si>
+  <si>
+    <t>Love Again</t>
+  </si>
+  <si>
+    <t>Wild</t>
+  </si>
+  <si>
+    <t>Is It True</t>
+  </si>
+  <si>
+    <t>The Seed (2.0)</t>
+  </si>
+  <si>
+    <t>The Roots ft Cody Chesnutt</t>
+  </si>
+  <si>
+    <t>Los Angeles</t>
+  </si>
+  <si>
+    <t>Dougie Poole</t>
+  </si>
+  <si>
+    <t>Crucifire</t>
+  </si>
+  <si>
+    <t>Desert Sessions</t>
+  </si>
+  <si>
+    <t>My Doorbell</t>
+  </si>
+  <si>
+    <t>The White Stripes</t>
+  </si>
+  <si>
+    <t>Judy Garland</t>
+  </si>
+  <si>
+    <t>Frog</t>
+  </si>
+  <si>
+    <t>Midnight City</t>
+  </si>
+  <si>
+    <t>M83</t>
+  </si>
+  <si>
+    <t>Scumbag Blues</t>
+  </si>
+  <si>
+    <t>Orange Crush</t>
+  </si>
+  <si>
+    <t>R.E.M.</t>
+  </si>
+  <si>
+    <t>Roscoe</t>
+  </si>
+  <si>
+    <t>Midlake</t>
+  </si>
+  <si>
+    <t>As It Was</t>
+  </si>
+  <si>
+    <t>Charli XCX</t>
+  </si>
+  <si>
+    <t>When Am I Gonna Lose You</t>
+  </si>
+  <si>
+    <t>Local Natives</t>
+  </si>
+  <si>
+    <t>The Bronze</t>
+  </si>
+  <si>
+    <t>Thinking of a Place</t>
+  </si>
+  <si>
+    <t>The War On Drugs</t>
+  </si>
+  <si>
+    <t>Wet Dream</t>
+  </si>
+  <si>
+    <t>Wet Leg</t>
+  </si>
+  <si>
+    <t>Naked in Manhattan</t>
+  </si>
+  <si>
+    <t>Dance Around It</t>
+  </si>
+  <si>
+    <t>Lucius ft Sheryl Crow, Brandi Carlile</t>
+  </si>
+  <si>
+    <t>In Too Deep</t>
+  </si>
+  <si>
+    <t>Slow Pulp</t>
+  </si>
+  <si>
+    <t>Little Death</t>
+  </si>
+  <si>
+    <t>The Beths</t>
+  </si>
+  <si>
+    <t>2 Be Loved (Am I Ready)</t>
+  </si>
+  <si>
+    <t>Clearest Blue</t>
+  </si>
+  <si>
+    <t>CHVRCHES</t>
+  </si>
+  <si>
+    <t>Ur Name on a Grain of Rice</t>
+  </si>
+  <si>
+    <t>Runnner</t>
+  </si>
+  <si>
+    <t>Want Want</t>
+  </si>
+  <si>
+    <t>Maggie Rogers</t>
+  </si>
+  <si>
+    <t>Hot Tub</t>
+  </si>
+  <si>
+    <t>Yung Gravy ft T-Pain, Dillon Francis</t>
+  </si>
+  <si>
+    <t>Solid</t>
+  </si>
+  <si>
+    <t>Fresh Fro</t>
+  </si>
+  <si>
+    <t>Exmiranda</t>
+  </si>
+  <si>
+    <t>Return of the Mack</t>
+  </si>
+  <si>
+    <t>Mark Morrison</t>
+  </si>
+  <si>
+    <t>Daytona Sand</t>
+  </si>
+  <si>
+    <t>Orville Peck</t>
+  </si>
+  <si>
+    <t>Summer's Here</t>
+  </si>
+  <si>
+    <t>James Taylor</t>
+  </si>
+  <si>
+    <t>Our House</t>
+  </si>
+  <si>
+    <t>Crosby, Stills, Nash &amp; Young</t>
+  </si>
+  <si>
+    <t>It's a good day (to fight the system)</t>
+  </si>
+  <si>
+    <t>Shungudzo</t>
+  </si>
+  <si>
+    <t>The King</t>
+  </si>
+  <si>
+    <t>Sarah Kinsley</t>
+  </si>
+  <si>
+    <t>Kissing Lessons</t>
+  </si>
+  <si>
+    <t>Witchoo</t>
+  </si>
+  <si>
+    <t>Durand Jones &amp; The Indications ft Aaron Frazer</t>
+  </si>
+  <si>
+    <t>Cold Heart - PNAU Remix</t>
+  </si>
+  <si>
+    <t>Elton John ft Dua Lipa, PNAU</t>
+  </si>
+  <si>
+    <t>Chaise Longue</t>
+  </si>
+  <si>
+    <t>Maybe You're The Problem</t>
+  </si>
+  <si>
+    <t>Ava Max</t>
   </si>
 </sst>
 </file>
@@ -3165,7 +3522,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="13.29"/>
     <col customWidth="1" min="2" max="2" width="38.29"/>
-    <col customWidth="1" min="3" max="3" width="32.43"/>
+    <col customWidth="1" min="3" max="3" width="71.57"/>
     <col customWidth="1" min="4" max="4" width="33.0"/>
     <col customWidth="1" min="5" max="5" width="13.29"/>
     <col customWidth="1" min="6" max="6" width="8.71"/>
@@ -3771,7 +4128,7 @@
       <c r="B23" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -4282,7 +4639,7 @@
       <c r="A42" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C42" s="2" t="s">
@@ -4309,7 +4666,7 @@
       <c r="A43" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="1" t="s">
         <v>89</v>
       </c>
       <c r="C43" s="2" t="s">
@@ -4525,7 +4882,7 @@
       <c r="A51" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="1" t="s">
         <v>103</v>
       </c>
       <c r="C51" s="2" t="s">
@@ -4687,7 +5044,7 @@
       <c r="A57" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C57" s="2" t="s">
@@ -4714,7 +5071,7 @@
       <c r="A58" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="1" t="s">
         <v>117</v>
       </c>
       <c r="C58" s="2" t="s">
@@ -14734,7 +15091,7 @@
       <c r="B429" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="C429" s="2" t="s">
+      <c r="C429" s="1" t="s">
         <v>737</v>
       </c>
       <c r="D429" s="2" t="s">
@@ -18056,7 +18413,7 @@
         <v>944</v>
       </c>
       <c r="C552" s="1" t="s">
-        <v>945</v>
+        <v>737</v>
       </c>
       <c r="D552" s="1" t="s">
         <v>880</v>
@@ -18080,10 +18437,10 @@
         <v>74</v>
       </c>
       <c r="B553" s="1" t="s">
+        <v>945</v>
+      </c>
+      <c r="C553" s="1" t="s">
         <v>946</v>
-      </c>
-      <c r="C553" s="1" t="s">
-        <v>947</v>
       </c>
       <c r="D553" s="1" t="s">
         <v>880</v>
@@ -18107,10 +18464,10 @@
         <v>74</v>
       </c>
       <c r="B554" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="C554" s="1" t="s">
         <v>948</v>
-      </c>
-      <c r="C554" s="1" t="s">
-        <v>949</v>
       </c>
       <c r="D554" s="1" t="s">
         <v>880</v>
@@ -18134,7 +18491,7 @@
         <v>74</v>
       </c>
       <c r="B555" s="1" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="C555" s="1" t="s">
         <v>620</v>
@@ -18161,10 +18518,10 @@
         <v>74</v>
       </c>
       <c r="B556" s="1" t="s">
+        <v>950</v>
+      </c>
+      <c r="C556" s="1" t="s">
         <v>951</v>
-      </c>
-      <c r="C556" s="1" t="s">
-        <v>952</v>
       </c>
       <c r="D556" s="1" t="s">
         <v>880</v>
@@ -18188,10 +18545,10 @@
         <v>74</v>
       </c>
       <c r="B557" s="1" t="s">
+        <v>952</v>
+      </c>
+      <c r="C557" s="1" t="s">
         <v>953</v>
-      </c>
-      <c r="C557" s="1" t="s">
-        <v>954</v>
       </c>
       <c r="D557" s="1" t="s">
         <v>880</v>
@@ -18215,10 +18572,10 @@
         <v>626</v>
       </c>
       <c r="B558" s="1" t="s">
+        <v>954</v>
+      </c>
+      <c r="C558" s="1" t="s">
         <v>955</v>
-      </c>
-      <c r="C558" s="1" t="s">
-        <v>956</v>
       </c>
       <c r="D558" s="1" t="s">
         <v>880</v>
@@ -18242,10 +18599,10 @@
         <v>626</v>
       </c>
       <c r="B559" s="1" t="s">
+        <v>956</v>
+      </c>
+      <c r="C559" s="1" t="s">
         <v>957</v>
-      </c>
-      <c r="C559" s="1" t="s">
-        <v>958</v>
       </c>
       <c r="D559" s="1" t="s">
         <v>880</v>
@@ -18269,7 +18626,7 @@
         <v>626</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="C560" s="1" t="s">
         <v>395</v>
@@ -18296,7 +18653,7 @@
         <v>626</v>
       </c>
       <c r="B561" s="1" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="C561" s="1" t="s">
         <v>913</v>
@@ -18323,10 +18680,10 @@
         <v>626</v>
       </c>
       <c r="B562" s="1" t="s">
+        <v>960</v>
+      </c>
+      <c r="C562" s="1" t="s">
         <v>961</v>
-      </c>
-      <c r="C562" s="1" t="s">
-        <v>962</v>
       </c>
       <c r="D562" s="1" t="s">
         <v>880</v>
@@ -18345,80 +18702,2004 @@
         <v>796</v>
       </c>
     </row>
-    <row r="563" ht="14.25" customHeight="1"/>
-    <row r="564" ht="14.25" customHeight="1"/>
-    <row r="565" ht="14.25" customHeight="1"/>
-    <row r="566" ht="14.25" customHeight="1"/>
-    <row r="567" ht="14.25" customHeight="1"/>
-    <row r="568" ht="14.25" customHeight="1"/>
-    <row r="569" ht="14.25" customHeight="1"/>
-    <row r="570" ht="14.25" customHeight="1"/>
-    <row r="571" ht="14.25" customHeight="1"/>
-    <row r="572" ht="14.25" customHeight="1"/>
-    <row r="573" ht="14.25" customHeight="1"/>
-    <row r="574" ht="14.25" customHeight="1"/>
-    <row r="575" ht="14.25" customHeight="1"/>
-    <row r="576" ht="14.25" customHeight="1"/>
-    <row r="577" ht="14.25" customHeight="1"/>
-    <row r="578" ht="14.25" customHeight="1"/>
-    <row r="579" ht="14.25" customHeight="1"/>
-    <row r="580" ht="14.25" customHeight="1"/>
-    <row r="581" ht="14.25" customHeight="1"/>
-    <row r="582" ht="14.25" customHeight="1"/>
-    <row r="583" ht="14.25" customHeight="1"/>
-    <row r="584" ht="14.25" customHeight="1"/>
-    <row r="585" ht="14.25" customHeight="1"/>
-    <row r="586" ht="14.25" customHeight="1"/>
-    <row r="587" ht="14.25" customHeight="1"/>
-    <row r="588" ht="14.25" customHeight="1"/>
-    <row r="589" ht="14.25" customHeight="1"/>
-    <row r="590" ht="14.25" customHeight="1"/>
-    <row r="591" ht="14.25" customHeight="1"/>
-    <row r="592" ht="14.25" customHeight="1"/>
-    <row r="593" ht="14.25" customHeight="1"/>
-    <row r="594" ht="14.25" customHeight="1"/>
-    <row r="595" ht="14.25" customHeight="1"/>
-    <row r="596" ht="14.25" customHeight="1"/>
-    <row r="597" ht="14.25" customHeight="1"/>
-    <row r="598" ht="14.25" customHeight="1"/>
-    <row r="599" ht="14.25" customHeight="1"/>
-    <row r="600" ht="14.25" customHeight="1"/>
-    <row r="601" ht="14.25" customHeight="1"/>
-    <row r="602" ht="14.25" customHeight="1"/>
-    <row r="603" ht="14.25" customHeight="1"/>
-    <row r="604" ht="14.25" customHeight="1"/>
-    <row r="605" ht="14.25" customHeight="1"/>
-    <row r="606" ht="14.25" customHeight="1"/>
-    <row r="607" ht="14.25" customHeight="1"/>
-    <row r="608" ht="14.25" customHeight="1"/>
-    <row r="609" ht="14.25" customHeight="1"/>
-    <row r="610" ht="14.25" customHeight="1"/>
-    <row r="611" ht="14.25" customHeight="1"/>
-    <row r="612" ht="14.25" customHeight="1"/>
-    <row r="613" ht="14.25" customHeight="1"/>
-    <row r="614" ht="14.25" customHeight="1"/>
-    <row r="615" ht="14.25" customHeight="1"/>
-    <row r="616" ht="14.25" customHeight="1"/>
-    <row r="617" ht="14.25" customHeight="1"/>
-    <row r="618" ht="14.25" customHeight="1"/>
-    <row r="619" ht="14.25" customHeight="1"/>
-    <row r="620" ht="14.25" customHeight="1"/>
-    <row r="621" ht="14.25" customHeight="1"/>
-    <row r="622" ht="14.25" customHeight="1"/>
-    <row r="623" ht="14.25" customHeight="1"/>
-    <row r="624" ht="14.25" customHeight="1"/>
-    <row r="625" ht="14.25" customHeight="1"/>
-    <row r="626" ht="14.25" customHeight="1"/>
-    <row r="627" ht="14.25" customHeight="1"/>
-    <row r="628" ht="14.25" customHeight="1"/>
-    <row r="629" ht="14.25" customHeight="1"/>
-    <row r="630" ht="14.25" customHeight="1"/>
-    <row r="631" ht="14.25" customHeight="1"/>
-    <row r="632" ht="14.25" customHeight="1"/>
-    <row r="633" ht="14.25" customHeight="1"/>
-    <row r="634" ht="14.25" customHeight="1"/>
-    <row r="635" ht="14.25" customHeight="1"/>
-    <row r="636" ht="14.25" customHeight="1"/>
+    <row r="563" ht="14.25" customHeight="1">
+      <c r="A563" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B563" s="1" t="s">
+        <v>962</v>
+      </c>
+      <c r="C563" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="D563" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E563" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F563" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E563)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G563" s="1">
+        <v>335.0</v>
+      </c>
+      <c r="H563" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="564" ht="14.25" customHeight="1">
+      <c r="A564" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B564" s="1" t="s">
+        <v>964</v>
+      </c>
+      <c r="C564" s="1" t="s">
+        <v>965</v>
+      </c>
+      <c r="D564" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E564" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F564" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E564)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G564" s="1">
+        <v>303.0</v>
+      </c>
+      <c r="H564" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="565" ht="14.25" customHeight="1">
+      <c r="A565" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B565" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C565" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="D565" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E565" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F565" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E565)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G565" s="1">
+        <v>354.0</v>
+      </c>
+      <c r="H565" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="566" ht="14.25" customHeight="1">
+      <c r="A566" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B566" s="1" t="s">
+        <v>966</v>
+      </c>
+      <c r="C566" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D566" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E566" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F566" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E566)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G566" s="1">
+        <v>359.0</v>
+      </c>
+      <c r="H566" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="567" ht="14.25" customHeight="1">
+      <c r="A567" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B567" s="1" t="s">
+        <v>967</v>
+      </c>
+      <c r="C567" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="D567" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E567" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F567" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E567)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G567" s="1">
+        <v>251.0</v>
+      </c>
+      <c r="H567" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="568" ht="14.25" customHeight="1">
+      <c r="A568" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B568" s="1" t="s">
+        <v>968</v>
+      </c>
+      <c r="C568" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="D568" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E568" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F568" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E568)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G568" s="1">
+        <v>336.0</v>
+      </c>
+      <c r="H568" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="569" ht="14.25" customHeight="1">
+      <c r="A569" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B569" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="C569" s="1" t="s">
+        <v>970</v>
+      </c>
+      <c r="D569" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E569" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F569" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E569)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G569" s="1">
+        <v>254.0</v>
+      </c>
+      <c r="H569" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="570" ht="14.25" customHeight="1">
+      <c r="A570" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B570" s="1" t="s">
+        <v>971</v>
+      </c>
+      <c r="C570" s="1" t="s">
+        <v>972</v>
+      </c>
+      <c r="D570" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E570" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F570" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E570)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G570" s="1">
+        <v>253.0</v>
+      </c>
+      <c r="H570" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="571" ht="14.25" customHeight="1">
+      <c r="A571" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B571" s="1" t="s">
+        <v>973</v>
+      </c>
+      <c r="C571" s="1" t="s">
+        <v>974</v>
+      </c>
+      <c r="D571" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E571" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F571" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E571)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G571" s="1">
+        <v>352.0</v>
+      </c>
+      <c r="H571" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="572" ht="14.25" customHeight="1">
+      <c r="A572" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B572" s="1" t="s">
+        <v>975</v>
+      </c>
+      <c r="C572" s="1" t="s">
+        <v>976</v>
+      </c>
+      <c r="D572" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E572" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F572" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E572)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G572" s="1">
+        <v>305.0</v>
+      </c>
+      <c r="H572" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="573" ht="14.25" customHeight="1">
+      <c r="A573" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B573" s="1" t="s">
+        <v>977</v>
+      </c>
+      <c r="C573" s="1" t="s">
+        <v>978</v>
+      </c>
+      <c r="D573" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E573" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F573" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E573)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G573" s="1">
+        <v>232.0</v>
+      </c>
+      <c r="H573" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="574" ht="14.25" customHeight="1">
+      <c r="A574" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B574" s="1" t="s">
+        <v>979</v>
+      </c>
+      <c r="C574" s="1" t="s">
+        <v>980</v>
+      </c>
+      <c r="D574" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E574" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F574" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E574)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G574" s="1">
+        <v>415.0</v>
+      </c>
+      <c r="H574" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="575" ht="14.25" customHeight="1">
+      <c r="A575" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B575" s="1" t="s">
+        <v>981</v>
+      </c>
+      <c r="C575" s="1" t="s">
+        <v>982</v>
+      </c>
+      <c r="D575" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E575" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F575" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E575)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G575" s="1">
+        <v>540.0</v>
+      </c>
+      <c r="H575" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="576" ht="14.25" customHeight="1">
+      <c r="A576" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B576" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="C576" s="1" t="s">
+        <v>984</v>
+      </c>
+      <c r="D576" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E576" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F576" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E576)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G576" s="1">
+        <v>343.0</v>
+      </c>
+      <c r="H576" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="577" ht="14.25" customHeight="1">
+      <c r="A577" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="B577" s="1" t="s">
+        <v>985</v>
+      </c>
+      <c r="C577" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="D577" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E577" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F577" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E577)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G577" s="1">
+        <v>452.0</v>
+      </c>
+      <c r="H577" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="578" ht="14.25" customHeight="1">
+      <c r="A578" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="B578" s="1" t="s">
+        <v>986</v>
+      </c>
+      <c r="C578" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="D578" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E578" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F578" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E578)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G578" s="1">
+        <v>627.0</v>
+      </c>
+      <c r="H578" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="579" ht="14.25" customHeight="1">
+      <c r="A579" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="B579" s="1" t="s">
+        <v>988</v>
+      </c>
+      <c r="C579" s="1" t="s">
+        <v>989</v>
+      </c>
+      <c r="D579" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E579" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F579" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E579)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G579" s="1">
+        <v>414.0</v>
+      </c>
+      <c r="H579" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="580" ht="14.25" customHeight="1">
+      <c r="A580" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="B580" s="1" t="s">
+        <v>990</v>
+      </c>
+      <c r="C580" s="1" t="s">
+        <v>991</v>
+      </c>
+      <c r="D580" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E580" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F580" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E580)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G580" s="1">
+        <v>301.0</v>
+      </c>
+      <c r="H580" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="581" ht="14.25" customHeight="1">
+      <c r="A581" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="B581" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="C581" s="1" t="s">
+        <v>970</v>
+      </c>
+      <c r="D581" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E581" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F581" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E581)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G581" s="1">
+        <v>313.0</v>
+      </c>
+      <c r="H581" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="582" ht="14.25" customHeight="1">
+      <c r="A582" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="B582" s="1" t="s">
+        <v>993</v>
+      </c>
+      <c r="C582" s="1" t="s">
+        <v>994</v>
+      </c>
+      <c r="D582" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E582" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F582" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E582)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G582" s="1">
+        <v>213.0</v>
+      </c>
+      <c r="H582" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="583" ht="14.25" customHeight="1">
+      <c r="A583" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B583" s="1" t="s">
+        <v>995</v>
+      </c>
+      <c r="C583" s="1" t="s">
+        <v>996</v>
+      </c>
+      <c r="D583" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E583" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F583" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E583)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G583" s="1">
+        <v>523.0</v>
+      </c>
+      <c r="H583" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="584" ht="14.25" customHeight="1">
+      <c r="A584" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B584" s="1" t="s">
+        <v>997</v>
+      </c>
+      <c r="C584" s="1" t="s">
+        <v>998</v>
+      </c>
+      <c r="D584" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E584" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F584" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E584)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G584" s="1">
+        <v>328.0</v>
+      </c>
+      <c r="H584" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="585" ht="14.25" customHeight="1">
+      <c r="A585" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B585" s="1" t="s">
+        <v>999</v>
+      </c>
+      <c r="C585" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D585" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E585" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F585" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E585)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G585" s="1">
+        <v>317.0</v>
+      </c>
+      <c r="H585" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="586" ht="14.25" customHeight="1">
+      <c r="A586" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B586" s="1" t="s">
+        <v>1001</v>
+      </c>
+      <c r="C586" s="1" t="s">
+        <v>1002</v>
+      </c>
+      <c r="D586" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E586" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F586" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E586)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G586" s="1">
+        <v>328.0</v>
+      </c>
+      <c r="H586" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="587" ht="14.25" customHeight="1">
+      <c r="A587" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B587" s="1" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C587" s="1" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D587" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E587" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F587" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E587)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G587" s="1">
+        <v>249.0</v>
+      </c>
+      <c r="H587" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="588" ht="14.25" customHeight="1">
+      <c r="A588" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B588" s="1" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C588" s="1" t="s">
+        <v>1006</v>
+      </c>
+      <c r="D588" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E588" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F588" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E588)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G588" s="1">
+        <v>323.0</v>
+      </c>
+      <c r="H588" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="589" ht="14.25" customHeight="1">
+      <c r="A589" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B589" s="1" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C589" s="1" t="s">
+        <v>1008</v>
+      </c>
+      <c r="D589" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E589" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F589" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E589)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G589" s="1">
+        <v>509.0</v>
+      </c>
+      <c r="H589" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="590" ht="14.25" customHeight="1">
+      <c r="A590" s="1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B590" s="1" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C590" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="D590" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E590" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F590" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E590)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G590" s="1">
+        <v>358.0</v>
+      </c>
+      <c r="H590" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="591" ht="14.25" customHeight="1">
+      <c r="A591" s="1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B591" s="1" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C591" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="D591" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E591" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F591" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E591)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G591" s="1">
+        <v>457.0</v>
+      </c>
+      <c r="H591" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="592" ht="14.25" customHeight="1">
+      <c r="A592" s="1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B592" s="1" t="s">
+        <v>1012</v>
+      </c>
+      <c r="C592" s="1" t="s">
+        <v>1013</v>
+      </c>
+      <c r="D592" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E592" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F592" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E592)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G592" s="1">
+        <v>313.0</v>
+      </c>
+      <c r="H592" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="593" ht="14.25" customHeight="1">
+      <c r="A593" s="1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B593" s="1" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C593" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="D593" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E593" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F593" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E593)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G593" s="1">
+        <v>418.0</v>
+      </c>
+      <c r="H593" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="594" ht="14.25" customHeight="1">
+      <c r="A594" s="1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B594" s="1" t="s">
+        <v>1015</v>
+      </c>
+      <c r="C594" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D594" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E594" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F594" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E594)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G594" s="1">
+        <v>313.0</v>
+      </c>
+      <c r="H594" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="595" ht="14.25" customHeight="1">
+      <c r="A595" s="1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B595" s="1" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C595" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D595" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E595" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F595" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E595)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G595" s="1">
+        <v>359.0</v>
+      </c>
+      <c r="H595" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="596" ht="14.25" customHeight="1">
+      <c r="A596" s="1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B596" s="1" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C596" s="1" t="s">
+        <v>1018</v>
+      </c>
+      <c r="D596" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E596" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F596" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E596)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G596" s="1">
+        <v>427.0</v>
+      </c>
+      <c r="H596" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="597" ht="14.25" customHeight="1">
+      <c r="A597" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B597" s="1" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C597" s="1" t="s">
+        <v>1020</v>
+      </c>
+      <c r="D597" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E597" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F597" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E597)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G597" s="1">
+        <v>437.0</v>
+      </c>
+      <c r="H597" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="598" ht="14.25" customHeight="1">
+      <c r="A598" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B598" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C598" s="1" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D598" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E598" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F598" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E598)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G598" s="1">
+        <v>144.0</v>
+      </c>
+      <c r="H598" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="599" ht="14.25" customHeight="1">
+      <c r="A599" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B599" s="1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C599" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D599" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E599" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F599" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E599)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G599" s="1">
+        <v>401.0</v>
+      </c>
+      <c r="H599" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="600" ht="14.25" customHeight="1">
+      <c r="A600" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B600" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="C600" s="1" t="s">
+        <v>835</v>
+      </c>
+      <c r="D600" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E600" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F600" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E600)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G600" s="1">
+        <v>320.0</v>
+      </c>
+      <c r="H600" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="601" ht="14.25" customHeight="1">
+      <c r="A601" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B601" s="1" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C601" s="1" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D601" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E601" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F601" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E601)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G601" s="1">
+        <v>337.0</v>
+      </c>
+      <c r="H601" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="602" ht="14.25" customHeight="1">
+      <c r="A602" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B602" s="1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C602" s="1" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D602" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E602" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F602" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E602)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G602" s="1">
+        <v>401.0</v>
+      </c>
+      <c r="H602" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="603" ht="14.25" customHeight="1">
+      <c r="A603" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B603" s="1" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C603" s="1" t="s">
+        <v>710</v>
+      </c>
+      <c r="D603" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E603" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F603" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E603)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G603" s="1">
+        <v>425.0</v>
+      </c>
+      <c r="H603" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="604" ht="14.25" customHeight="1">
+      <c r="A604" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B604" s="1" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C604" s="1" t="s">
+        <v>1031</v>
+      </c>
+      <c r="D604" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E604" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F604" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E604)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G604" s="1">
+        <v>351.0</v>
+      </c>
+      <c r="H604" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="605" ht="14.25" customHeight="1">
+      <c r="A605" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B605" s="1" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C605" s="1" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D605" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E605" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F605" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E605)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G605" s="1">
+        <v>446.0</v>
+      </c>
+      <c r="H605" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="606" ht="14.25" customHeight="1">
+      <c r="A606" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B606" s="1" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C606" s="1" t="s">
+        <v>970</v>
+      </c>
+      <c r="D606" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E606" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F606" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E606)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G606" s="1">
+        <v>247.0</v>
+      </c>
+      <c r="H606" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="607" ht="14.25" customHeight="1">
+      <c r="A607" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B607" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="C607" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="D607" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E607" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F607" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E607)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G607" s="1">
+        <v>325.0</v>
+      </c>
+      <c r="H607" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="608" ht="14.25" customHeight="1">
+      <c r="A608" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B608" s="1" t="s">
+        <v>1015</v>
+      </c>
+      <c r="C608" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D608" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E608" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F608" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E608)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G608" s="1">
+        <v>313.0</v>
+      </c>
+      <c r="H608" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="609" ht="14.25" customHeight="1">
+      <c r="A609" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B609" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C609" s="1" t="s">
+        <v>1035</v>
+      </c>
+      <c r="D609" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E609" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F609" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E609)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G609" s="1">
+        <v>218.0</v>
+      </c>
+      <c r="H609" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="610" ht="14.25" customHeight="1">
+      <c r="A610" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B610" s="1" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C610" s="1" t="s">
+        <v>1037</v>
+      </c>
+      <c r="D610" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E610" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F610" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E610)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G610" s="1">
+        <v>424.0</v>
+      </c>
+      <c r="H610" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="611" ht="14.25" customHeight="1">
+      <c r="A611" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B611" s="1" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C611" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D611" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E611" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F611" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E611)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G611" s="1">
+        <v>345.0</v>
+      </c>
+      <c r="H611" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="612" ht="14.25" customHeight="1">
+      <c r="A612" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B612" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="C612" s="1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="D612" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E612" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F612" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E612)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G612" s="1">
+        <v>1110.0</v>
+      </c>
+      <c r="H612" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="613" ht="14.25" customHeight="1">
+      <c r="A613" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="B613" s="1" t="s">
+        <v>1041</v>
+      </c>
+      <c r="C613" s="1" t="s">
+        <v>1042</v>
+      </c>
+      <c r="D613" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E613" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F613" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E613)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G613" s="1">
+        <v>220.0</v>
+      </c>
+      <c r="H613" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="614" ht="14.25" customHeight="1">
+      <c r="A614" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="B614" s="1" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C614" s="1" t="s">
+        <v>928</v>
+      </c>
+      <c r="D614" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E614" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F614" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E614)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G614" s="1">
+        <v>331.0</v>
+      </c>
+      <c r="H614" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="615" ht="14.25" customHeight="1">
+      <c r="A615" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="B615" s="1" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C615" s="1" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D615" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E615" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F615" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E615)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G615" s="1">
+        <v>326.0</v>
+      </c>
+      <c r="H615" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="616" ht="14.25" customHeight="1">
+      <c r="A616" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="B616" s="1" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C616" s="1" t="s">
+        <v>1047</v>
+      </c>
+      <c r="D616" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E616" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F616" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E616)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G616" s="1">
+        <v>341.0</v>
+      </c>
+      <c r="H616" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="617" ht="14.25" customHeight="1">
+      <c r="A617" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="B617" s="1" t="s">
+        <v>1048</v>
+      </c>
+      <c r="C617" s="1" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D617" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E617" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F617" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E617)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G617" s="1">
+        <v>454.0</v>
+      </c>
+      <c r="H617" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="618" ht="14.25" customHeight="1">
+      <c r="A618" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="B618" s="1" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C618" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="D618" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E618" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F618" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E618)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G618" s="1">
+        <v>307.0</v>
+      </c>
+      <c r="H618" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="619" ht="14.25" customHeight="1">
+      <c r="A619" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="B619" s="1" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C619" s="1" t="s">
+        <v>1052</v>
+      </c>
+      <c r="D619" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E619" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F619" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E619)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G619" s="1">
+        <v>353.0</v>
+      </c>
+      <c r="H619" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="620" ht="14.25" customHeight="1">
+      <c r="A620" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="B620" s="1" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C620" s="1" t="s">
+        <v>1054</v>
+      </c>
+      <c r="D620" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E620" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F620" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E620)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G620" s="1">
+        <v>501.0</v>
+      </c>
+      <c r="H620" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="621" ht="14.25" customHeight="1">
+      <c r="A621" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B621" s="1" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C621" s="1" t="s">
+        <v>1056</v>
+      </c>
+      <c r="D621" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E621" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F621" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E621)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G621" s="1">
+        <v>308.0</v>
+      </c>
+      <c r="H621" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="622" ht="14.25" customHeight="1">
+      <c r="A622" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B622" s="1" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C622" s="1" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D622" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E622" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F622" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E622)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G622" s="1">
+        <v>239.0</v>
+      </c>
+      <c r="H622" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="623" ht="14.25" customHeight="1">
+      <c r="A623" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B623" s="1" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C623" s="1" t="s">
+        <v>953</v>
+      </c>
+      <c r="D623" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E623" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F623" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E623)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G623" s="1">
+        <v>221.0</v>
+      </c>
+      <c r="H623" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="624" ht="14.25" customHeight="1">
+      <c r="A624" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B624" s="1" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C624" s="1" t="s">
+        <v>1061</v>
+      </c>
+      <c r="D624" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E624" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F624" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E624)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G624" s="1">
+        <v>355.0</v>
+      </c>
+      <c r="H624" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="625" ht="14.25" customHeight="1">
+      <c r="A625" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B625" s="1" t="s">
+        <v>1062</v>
+      </c>
+      <c r="C625" s="1" t="s">
+        <v>1063</v>
+      </c>
+      <c r="D625" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E625" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F625" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E625)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G625" s="1">
+        <v>333.0</v>
+      </c>
+      <c r="H625" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="626" ht="14.25" customHeight="1">
+      <c r="A626" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B626" s="1" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C626" s="1" t="s">
+        <v>1065</v>
+      </c>
+      <c r="D626" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E626" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F626" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E626)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G626" s="1">
+        <v>315.0</v>
+      </c>
+      <c r="H626" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="627" ht="14.25" customHeight="1">
+      <c r="A627" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B627" s="1" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C627" s="1" t="s">
+        <v>1067</v>
+      </c>
+      <c r="D627" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E627" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F627" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E627)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G627" s="1">
+        <v>242.0</v>
+      </c>
+      <c r="H627" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="628" ht="14.25" customHeight="1">
+      <c r="A628" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B628" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C628" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D628" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E628" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F628" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E628)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G628" s="1">
+        <v>337.0</v>
+      </c>
+      <c r="H628" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="629" ht="14.25" customHeight="1">
+      <c r="A629" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="B629" s="1" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C629" s="1" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D629" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E629" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F629" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E629)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G629" s="1">
+        <v>259.0</v>
+      </c>
+      <c r="H629" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="630" ht="14.25" customHeight="1">
+      <c r="A630" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="B630" s="1" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C630" s="1" t="s">
+        <v>1071</v>
+      </c>
+      <c r="D630" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E630" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F630" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E630)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G630" s="1">
+        <v>317.0</v>
+      </c>
+      <c r="H630" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="631" ht="14.25" customHeight="1">
+      <c r="A631" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="B631" s="1" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C631" s="1" t="s">
+        <v>1073</v>
+      </c>
+      <c r="D631" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E631" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F631" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E631)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G631" s="1">
+        <v>326.0</v>
+      </c>
+      <c r="H631" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="632" ht="14.25" customHeight="1">
+      <c r="A632" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="B632" s="1" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C632" s="1" t="s">
+        <v>957</v>
+      </c>
+      <c r="D632" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E632" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F632" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E632)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G632" s="1">
+        <v>154.0</v>
+      </c>
+      <c r="H632" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="633" ht="14.25" customHeight="1">
+      <c r="A633" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="B633" s="1" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C633" s="1" t="s">
+        <v>1076</v>
+      </c>
+      <c r="D633" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E633" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F633" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E633)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G633" s="1">
+        <v>342.0</v>
+      </c>
+      <c r="H633" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="634" ht="14.25" customHeight="1">
+      <c r="A634" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="B634" s="1" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C634" s="1" t="s">
+        <v>1078</v>
+      </c>
+      <c r="D634" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E634" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F634" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E634)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G634" s="1">
+        <v>322.0</v>
+      </c>
+      <c r="H634" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="635" ht="14.25" customHeight="1">
+      <c r="A635" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="B635" s="1" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C635" s="1" t="s">
+        <v>1042</v>
+      </c>
+      <c r="D635" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E635" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F635" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E635)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G635" s="1">
+        <v>316.0</v>
+      </c>
+      <c r="H635" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="636" ht="14.25" customHeight="1">
+      <c r="A636" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="B636" s="1" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C636" s="1" t="s">
+        <v>1081</v>
+      </c>
+      <c r="D636" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E636" s="1">
+        <v>2022.0</v>
+      </c>
+      <c r="F636" s="2" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TO_TEXT(E636)"),"2022")</f>
+        <v>2022</v>
+      </c>
+      <c r="G636" s="1">
+        <v>310.0</v>
+      </c>
+      <c r="H636" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
     <row r="637" ht="14.25" customHeight="1"/>
     <row r="638" ht="14.25" customHeight="1"/>
     <row r="639" ht="14.25" customHeight="1"/>

</xml_diff>